<commit_message>
Added output raw data files for importing into matlab
Signed-off-by: Ethan Tola <ext9285@g.rit.edu>
</commit_message>
<xml_diff>
--- a/docs/Schedule_Task_Book.xlsx
+++ b/docs/Schedule_Task_Book.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Shared\Ravven Labs Ethan\april-tag-baseline\windows-c-code\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Ravven Labs Ethan\ravven-tag\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC59E56-DD9A-4FB4-A6AB-37EE4D3EAC3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14AC9CF-65B4-4BCF-84A8-7241F386A060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4680F21B-093D-46A3-8DBF-E9415BE66171}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{4680F21B-093D-46A3-8DBF-E9415BE66171}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Task</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>Create a word doc to contain a "journal" of everything</t>
+  </si>
+  <si>
+    <t>Almost, some timings need to be adjusted as they're done quickly.</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Output the data from each step in C</t>
   </si>
 </sst>
 </file>
@@ -450,7 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5897B7-0214-4CE3-8793-C931797A8330}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -497,96 +506,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909A5505-4CB2-4AC8-AA96-D1F767A6CF9F}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="51" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>